<commit_message>
nmi not generated. investigate...
</commit_message>
<xml_diff>
--- a/doc/debug-work.xlsx
+++ b/doc/debug-work.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="405" windowWidth="27795" windowHeight="12285"/>
+    <workbookView xWindow="600" yWindow="405" windowWidth="27795" windowHeight="12285" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="clock calc" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="135">
   <si>
     <t>---DE1 base clock 50 MHz</t>
   </si>
@@ -502,7 +502,107 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>2612E1</t>
+    <t>25ED60</t>
+  </si>
+  <si>
+    <t>&gt;&gt; nmi ok.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>#3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2C5600</t>
+  </si>
+  <si>
+    <t>&gt;&gt;ok</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>#4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>32BEA0</t>
+  </si>
+  <si>
+    <t>&gt;ok</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>#5</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>392740</t>
+  </si>
+  <si>
+    <t>#10</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>5F9B00</t>
+  </si>
+  <si>
+    <t>7FA620</t>
+  </si>
+  <si>
+    <t>#20</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>#30</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>#25</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ng</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>#26</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>#27</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>#28</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>&lt;&lt;&lt;wrong!!!</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>clock=</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>B2EB20</t>
+  </si>
+  <si>
+    <t>AC8280</t>
+  </si>
+  <si>
+    <t>A619E0</t>
+  </si>
+  <si>
+    <t>#28 case</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -780,6 +880,53 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="26574750"/>
+          <a:ext cx="18288000" cy="10287000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>248</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>308</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="685800" y="42519600"/>
           <a:ext cx="18288000" cy="10287000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3035,7 +3182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -3246,19 +3393,19 @@
         <v>19</v>
       </c>
       <c r="C29" s="10">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="G29" t="s">
-        <v>105</v>
+      <c r="G29">
+        <v>241264</v>
       </c>
     </row>
     <row r="30" spans="2:10">
       <c r="B30" t="str">
         <f>C29&amp;"回目のvblankは"</f>
-        <v>3回目のvblankは</v>
+        <v>26回目のvblankは</v>
       </c>
       <c r="F30" t="s">
         <v>20</v>
@@ -3267,7 +3414,7 @@
     <row r="31" spans="2:10">
       <c r="C31" s="5">
         <f>G27 + $C$26*(C29-1)</f>
-        <v>1225600</v>
+        <v>10885600</v>
       </c>
       <c r="D31" s="1"/>
       <c r="F31" t="s">
@@ -3275,21 +3422,21 @@
       </c>
       <c r="G31" s="1">
         <f>HEX2DEC(G29)</f>
-        <v>1225745</v>
+        <v>2364004</v>
       </c>
       <c r="I31" s="5"/>
     </row>
     <row r="32" spans="2:10">
       <c r="C32" s="11" t="str">
         <f>DEC2HEX(C31)</f>
-        <v>12B380</v>
+        <v>A619E0</v>
       </c>
       <c r="D32" t="s">
         <v>100</v>
       </c>
       <c r="G32" s="11">
         <f>ROUND(G31/C26,1)</f>
-        <v>2.9</v>
+        <v>5.6</v>
       </c>
       <c r="H32" t="s">
         <v>22</v>
@@ -3304,10 +3451,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:N220"/>
+  <dimension ref="A3:N248"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" topLeftCell="A250" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B249" sqref="B249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3576,7 +3723,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="219" spans="1:4">
+    <row r="219" spans="1:5">
       <c r="A219" t="s">
         <v>96</v>
       </c>
@@ -3584,7 +3731,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="220" spans="1:4">
+    <row r="220" spans="1:5">
       <c r="A220" t="s">
         <v>91</v>
       </c>
@@ -3596,6 +3743,188 @@
       </c>
       <c r="D220" t="s">
         <v>106</v>
+      </c>
+      <c r="E220" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5">
+      <c r="A223" t="s">
+        <v>109</v>
+      </c>
+      <c r="B223" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5">
+      <c r="A224" t="s">
+        <v>91</v>
+      </c>
+      <c r="B224" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C224" t="s">
+        <v>89</v>
+      </c>
+      <c r="D224" t="s">
+        <v>106</v>
+      </c>
+      <c r="E224" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4">
+      <c r="A227" t="s">
+        <v>112</v>
+      </c>
+      <c r="B227" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4">
+      <c r="A228" t="s">
+        <v>91</v>
+      </c>
+      <c r="B228" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C228" t="s">
+        <v>89</v>
+      </c>
+      <c r="D228" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4">
+      <c r="A231" t="s">
+        <v>115</v>
+      </c>
+      <c r="B231" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4">
+      <c r="A232" t="s">
+        <v>91</v>
+      </c>
+      <c r="B232" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C232" t="s">
+        <v>89</v>
+      </c>
+      <c r="D232" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4">
+      <c r="A235" t="s">
+        <v>117</v>
+      </c>
+      <c r="B235" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4">
+      <c r="A236" t="s">
+        <v>91</v>
+      </c>
+      <c r="B236" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C236" t="s">
+        <v>89</v>
+      </c>
+      <c r="D236" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4">
+      <c r="A239" t="s">
+        <v>120</v>
+      </c>
+      <c r="B239" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4">
+      <c r="A240" t="s">
+        <v>91</v>
+      </c>
+      <c r="B240" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C240" t="s">
+        <v>89</v>
+      </c>
+      <c r="D240" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6">
+      <c r="A242" t="s">
+        <v>123</v>
+      </c>
+      <c r="B242" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6">
+      <c r="A243" t="s">
+        <v>126</v>
+      </c>
+      <c r="B243" t="s">
+        <v>124</v>
+      </c>
+      <c r="E243" t="s">
+        <v>130</v>
+      </c>
+      <c r="F243" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6">
+      <c r="A244" t="s">
+        <v>127</v>
+      </c>
+      <c r="B244" t="s">
+        <v>124</v>
+      </c>
+      <c r="E244" t="s">
+        <v>130</v>
+      </c>
+      <c r="F244" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6">
+      <c r="A245" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B245" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C245" t="s">
+        <v>129</v>
+      </c>
+      <c r="E245" t="s">
+        <v>130</v>
+      </c>
+      <c r="F245" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6">
+      <c r="A246" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B246" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6">
+      <c r="B248" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debug work doc added
</commit_message>
<xml_diff>
--- a/doc/debug-work.xlsx
+++ b/doc/debug-work.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motooka\Documents\001-proj\999.my-proj\001.nes-fpga\repo\motonesfpga\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="405" windowWidth="27795" windowHeight="12285" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="405" windowWidth="27795" windowHeight="12285" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="clock calc" sheetId="1" r:id="rId1"/>
     <sheet name="smb debug" sheetId="3" r:id="rId2"/>
+    <sheet name="emu-info" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="183">
   <si>
     <t>---DE1 base clock 50 MHz</t>
   </si>
@@ -393,16 +399,305 @@
     <t>#28 case</t>
     <phoneticPr fontId="2"/>
   </si>
+  <si>
+    <t>nmi</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>回目</t>
+  </si>
+  <si>
+    <t>BGなし</t>
+  </si>
+  <si>
+    <t>1c</t>
+  </si>
+  <si>
+    <t>BGのみ</t>
+  </si>
+  <si>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>BG+Spr</t>
+  </si>
+  <si>
+    <t>1e</t>
+  </si>
+  <si>
+    <t>sprite hit @(90, 29)</t>
+  </si>
+  <si>
+    <t>motonesemu start...</t>
+  </si>
+  <si>
+    <t>joypad key entry:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    select button:  &lt;Tab&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    start button:   &lt;Enter&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    up key:         Q, W, E, R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    down key:       Z, X, C, V, B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    left key:       A, S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    right key:      D, F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    A button:       &lt;:&gt;, &lt;]&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    B button:       L, &lt;;&gt;</t>
+  </si>
+  <si>
+    <t>cpu clock started.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8000: 78          SEI   </t>
+  </si>
+  <si>
+    <t>motonesemu: motonesemu: motonesemu: motonesemu: 1b00000000000000</t>
+  </si>
+  <si>
+    <t>1b, 0</t>
+  </si>
+  <si>
+    <t>motonesemu: motonesemu: ------------------</t>
+  </si>
+  <si>
+    <t>break...</t>
+  </si>
+  <si>
+    <t>clock: 1b00000000000000</t>
+  </si>
+  <si>
+    <t>6502 CPU registers:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pc:     8082</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> acc:    90</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> x:      ff</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> y:      ff</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sp:     fc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> status:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  negative:   1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  overflow:   0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  break:      0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  decimal:    0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  irq:        1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  zero:       0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  carry:      1</t>
+  </si>
+  <si>
+    <t>-------------------</t>
+  </si>
+  <si>
+    <t>1b00000000000000 8082: ad 78 07    LDA   $0778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0010: f8 00 00 00 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0020: f8 00 00 00 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0030: f8 00 00 00 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0040: f8 00 00 00 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0050: f8 00 00 00 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0060: f8 00 00 00 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0070: f8 00 00 00 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0080: f8 00 00 00 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0090: f8 00 00 00 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00a0: f8 00 00 00 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00b0: f8 00 00 00 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00c0: f8 00 00 00 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00d0: f8 00 00 00 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00e0: f8 00 00 00 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00f0: f8 00 00 00 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <t>motonesemu: 1c00000000000000</t>
+  </si>
+  <si>
+    <t>1c, 0</t>
+  </si>
+  <si>
+    <t>motonesemu: motonesemu: sprite hit @(89, 29)</t>
+  </si>
+  <si>
+    <t>sprite hit @(91, 29)</t>
+  </si>
+  <si>
+    <t>sprite hit @(92, 29)</t>
+  </si>
+  <si>
+    <t>sprite hit @(93, 29)</t>
+  </si>
+  <si>
+    <t>sprite hit @(90, 30)</t>
+  </si>
+  <si>
+    <t>sprite hit @(91, 30)</t>
+  </si>
+  <si>
+    <t>sprite hit @(92, 30)</t>
+  </si>
+  <si>
+    <t>------------------</t>
+  </si>
+  <si>
+    <t>clock: 1c00000000000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> x:      05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> y:      00</t>
+  </si>
+  <si>
+    <t>1c00000000000000 8082: ad 78 07    LDA   $0778</t>
+  </si>
+  <si>
+    <t>motonesemu: 1d00000000000000</t>
+  </si>
+  <si>
+    <t>1d, 0</t>
+  </si>
+  <si>
+    <t>clock: 1d00000000000000</t>
+  </si>
+  <si>
+    <t>1d00000000000000 8082: ad 78 07    LDA   $0778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0010: b8 fc 00 30 c0 3a 00 28   c0 37 00 30 c8 4f 00 28 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0020: c8 4f 40 30 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <t>motonesemu: 1e00000000000000</t>
+  </si>
+  <si>
+    <t>1e, 0</t>
+  </si>
+  <si>
+    <t>clock: 1e00000000000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> y:      05</t>
+  </si>
+  <si>
+    <t>1e00000000000000 8082: ad 78 07    LDA   $0778</t>
+  </si>
+  <si>
+    <t>motonesemu: quit...</t>
+  </si>
+  <si>
+    <t>clean data...</t>
+  </si>
+  <si>
+    <t>cpu clock thread joined.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000: f8 00 00 00 f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0000: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>18 ff 23 58</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve"> f8 00 00 00   f8 00 00 00 f8 00 00 00 </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">0000: 18 ff 23 58 b0 fc 00 28   b0 fc 00 30 b8 fc 00 28 </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -410,14 +705,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -425,7 +720,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -434,7 +729,7 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -443,10 +738,24 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="3">
@@ -480,7 +789,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -514,10 +823,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="桁区切り" xfId="1" builtinId="6"/>
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -725,8 +1037,171 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangular Callout 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4810125" y="10001250"/>
+          <a:ext cx="1352550" cy="847725"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -95481"/>
+            <a:gd name="adj2" fmla="val 81601"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>1b</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>の</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>nmi</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>で</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>DMA</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>して</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>sprite</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>を設定していると思う。</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangular Callout 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="190500"/>
+          <a:ext cx="1352550" cy="847725"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -134213"/>
+            <a:gd name="adj2" fmla="val -16152"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>sprite</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>0</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>のみ設定</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -768,7 +1243,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -800,9 +1275,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -834,6 +1310,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1009,23 +1486,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11.875" customWidth="1"/>
-    <col min="3" max="3" width="13.375" customWidth="1"/>
-    <col min="4" max="4" width="12.125" customWidth="1"/>
-    <col min="5" max="5" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.125" customWidth="1"/>
-    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.375" customWidth="1"/>
-    <col min="9" max="9" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6">
@@ -1218,7 +1695,7 @@
         <v>420000</v>
       </c>
     </row>
-    <row r="29" spans="2:10" ht="18.75">
+    <row r="29" spans="2:10" ht="21">
       <c r="B29" s="8" t="s">
         <v>19</v>
       </c>
@@ -1280,14 +1757,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A230" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A269" sqref="A269"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
@@ -1762,4 +2239,1025 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F202"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2">
+        <f>(HEX2DEC(B2))</f>
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3">
+        <f>(HEX2DEC(B3))</f>
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <f>(HEX2DEC(B4))</f>
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5">
+        <f>(HEX2DEC(B5))</f>
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2">
+      <c r="B64" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2">
+      <c r="B80" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" s="11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2">
+      <c r="B90" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2">
+      <c r="B91" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2">
+      <c r="B93" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2">
+      <c r="B94" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2">
+      <c r="B95" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2">
+      <c r="B96" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2">
+      <c r="B101" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2">
+      <c r="B102" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2">
+      <c r="B104" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2">
+      <c r="B106" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2">
+      <c r="B107" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2">
+      <c r="B108" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2">
+      <c r="B109" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2">
+      <c r="B110" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2">
+      <c r="B111" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2">
+      <c r="B112" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2">
+      <c r="B113" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2">
+      <c r="B114" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2">
+      <c r="B115" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2">
+      <c r="B116" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2">
+      <c r="B117" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2">
+      <c r="B119" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2">
+      <c r="B120" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2">
+      <c r="B121" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2">
+      <c r="B122" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2">
+      <c r="B123" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2">
+      <c r="B124" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2">
+      <c r="B125" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2">
+      <c r="B126" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2">
+      <c r="B127" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2">
+      <c r="B128" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2">
+      <c r="B129" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2">
+      <c r="B130" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2">
+      <c r="B131" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2">
+      <c r="B132" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2">
+      <c r="B133" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2">
+      <c r="B134" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2">
+      <c r="B135" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2">
+      <c r="B136" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2">
+      <c r="B137" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2">
+      <c r="B138" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2">
+      <c r="B139" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2">
+      <c r="B140" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2">
+      <c r="B141" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2">
+      <c r="B142" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2">
+      <c r="B143" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2">
+      <c r="B144" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2">
+      <c r="B145" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2">
+      <c r="B146" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2">
+      <c r="B147" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2">
+      <c r="B148" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2">
+      <c r="B149" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2">
+      <c r="B150" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2">
+      <c r="B151" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2">
+      <c r="B153" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2">
+      <c r="B154" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2">
+      <c r="B155" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2">
+      <c r="B156" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2">
+      <c r="B157" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2">
+      <c r="B158" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2">
+      <c r="B159" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2">
+      <c r="B160" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2">
+      <c r="B161" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2">
+      <c r="B162" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2">
+      <c r="B163" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2">
+      <c r="B164" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2">
+      <c r="B166" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2">
+      <c r="B167" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2">
+      <c r="B168" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2">
+      <c r="B169" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="170" spans="2:2">
+      <c r="B170" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2">
+      <c r="B171" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="172" spans="2:2">
+      <c r="B172" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="173" spans="2:2">
+      <c r="B173" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="174" spans="2:2">
+      <c r="B174" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="175" spans="2:2">
+      <c r="B175" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="176" spans="2:2">
+      <c r="B176" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="177" spans="2:2">
+      <c r="B177" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="178" spans="2:2">
+      <c r="B178" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="179" spans="2:2">
+      <c r="B179" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="180" spans="2:2">
+      <c r="B180" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="181" spans="2:2">
+      <c r="B181" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="182" spans="2:2">
+      <c r="B182" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="183" spans="2:2">
+      <c r="B183" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="2:2">
+      <c r="B184" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="185" spans="2:2">
+      <c r="B185" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="186" spans="2:2">
+      <c r="B186" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="187" spans="2:2">
+      <c r="B187" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="188" spans="2:2">
+      <c r="B188" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="189" spans="2:2">
+      <c r="B189" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2">
+      <c r="B190" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="191" spans="2:2">
+      <c r="B191" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="192" spans="2:2">
+      <c r="B192" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2">
+      <c r="B193" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="194" spans="2:2">
+      <c r="B194" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="195" spans="2:2">
+      <c r="B195" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="196" spans="2:2">
+      <c r="B196" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="197" spans="2:2">
+      <c r="B197" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="198" spans="2:2">
+      <c r="B198" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="200" spans="2:2">
+      <c r="B200" s="11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="201" spans="2:2">
+      <c r="B201" s="11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="202" spans="2:2">
+      <c r="B202" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>